<commit_message>
7 Oct 2023 Selenium Goibibo App
</commit_message>
<xml_diff>
--- a/Materials/Selenium Assignments by Raghuveer.xlsx
+++ b/Materials/Selenium Assignments by Raghuveer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\-SSJuneSeleniumJava2023\src\test\resources\Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\AugSeleniumJava2023\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9CC6E8-45B6-497D-A2D4-919BD3A64C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB88F07-0226-49E7-B96B-DCB46A26FEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -703,6 +703,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -924,8 +927,8 @@
   </sheetPr>
   <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5"/>
@@ -1268,7 +1271,7 @@
       <c r="C10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="17" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="1"/>

</xml_diff>